<commit_message>
IfoCAST evaluation development, some bugs remain
</commit_message>
<xml_diff>
--- a/0_0_Data/0_Forecast_Inputs/ifoForecast_dates.xlsx
+++ b/0_0_Data/0_Forecast_Inputs/ifoForecast_dates.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="8_{65D895AF-2E5F-4AD9-BE86-B11F0C995532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{993507BD-7A1B-4294-910D-C94971DB033B}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="19360" windowHeight="10960" xr2:uid="{418722FF-C76C-44D2-90A5-3603EF54561B}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="11170" xr2:uid="{418722FF-C76C-44D2-90A5-3603EF54561B}"/>
   </bookViews>
   <sheets>
     <sheet name="Veröffentlichungstermine" sheetId="1" r:id="rId1"/>
@@ -279,6 +279,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -604,7 +608,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected some selection scopes
</commit_message>
<xml_diff>
--- a/0_0_Data/0_Forecast_Inputs/ifoForecast_dates.xlsx
+++ b/0_0_Data/0_Forecast_Inputs/ifoForecast_dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/0_0_Data/0_Forecast_Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{65D895AF-2E5F-4AD9-BE86-B11F0C995532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{993507BD-7A1B-4294-910D-C94971DB033B}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{65D895AF-2E5F-4AD9-BE86-B11F0C995532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96C9B62C-3DB2-4C13-BE2A-6A4DD31024CA}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="11170" xr2:uid="{418722FF-C76C-44D2-90A5-3603EF54561B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{418722FF-C76C-44D2-90A5-3603EF54561B}"/>
   </bookViews>
   <sheets>
     <sheet name="Veröffentlichungstermine" sheetId="1" r:id="rId1"/>
@@ -279,10 +279,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -604,11 +600,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB973F84-AE58-48DD-AE4F-711C7A634A32}">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1754,14 +1750,14 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" si="2"/>
         <v>2020</v>
       </c>
       <c r="D65" s="2">
-        <v>44013</v>
+        <v>44011</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>5</v>

</xml_diff>